<commit_message>
Klasa tworząca okna, optymalizacja ilości kodu
</commit_message>
<xml_diff>
--- a/Plan zadań.xlsx
+++ b/Plan zadań.xlsx
@@ -458,7 +458,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,7 +563,7 @@
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -583,7 +583,7 @@
       <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -787,10 +787,10 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="A23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -807,18 +807,18 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Klasa weryfikująca poprawność danych, edycja produktów
</commit_message>
<xml_diff>
--- a/Plan zadań.xlsx
+++ b/Plan zadań.xlsx
@@ -458,7 +458,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,7 +537,7 @@
       <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -563,7 +563,7 @@
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -608,7 +608,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -617,10 +617,10 @@
       <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="4" t="s">
+      <c r="G9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Usuwanie produktu, sprawdzony panel pracownika
</commit_message>
<xml_diff>
--- a/Plan zadań.xlsx
+++ b/Plan zadań.xlsx
@@ -112,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,12 +143,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -162,12 +156,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -458,7 +451,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,32 +467,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
       <c r="E1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="M3" s="6" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="M3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -583,7 +576,7 @@
       <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -625,19 +618,19 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
@@ -657,114 +650,114 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="5"/>
+      <c r="C14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="4"/>
       <c r="K14" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="4"/>
+      <c r="G15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5" t="s">
+      <c r="H15" s="4"/>
+      <c r="I15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5" t="s">
+      <c r="H16" s="4"/>
+      <c r="I16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
@@ -790,13 +783,13 @@
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -807,13 +800,13 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>